<commit_message>
Made final review and final changes.
</commit_message>
<xml_diff>
--- a/documents/Gantt Chart - Job Satisfaction Dashboard.xlsx
+++ b/documents/Gantt Chart - Job Satisfaction Dashboard.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\New Computer Owner\Documents\Data Science MASTERS\Capstone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\New Computer Owner\Documents\Data Science MASTERS\Capstone\capstone-lawson\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FEE379-5FF0-48A5-BB89-98CBE68C2615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620B41E1-2076-4FD0-B80A-87146C2024AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project schedule" sheetId="11" r:id="rId1"/>
@@ -1147,14 +1147,20 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1171,20 +1177,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="166" fontId="18" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1816,28 +1816,28 @@
       <c r="E1" s="20"/>
       <c r="F1" s="21"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="117" t="s">
+      <c r="I1" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="118"/>
-      <c r="K1" s="118"/>
-      <c r="L1" s="118"/>
-      <c r="M1" s="118"/>
-      <c r="N1" s="118"/>
-      <c r="O1" s="118"/>
+      <c r="J1" s="120"/>
+      <c r="K1" s="120"/>
+      <c r="L1" s="120"/>
+      <c r="M1" s="120"/>
+      <c r="N1" s="120"/>
+      <c r="O1" s="120"/>
       <c r="P1" s="24"/>
-      <c r="Q1" s="116">
+      <c r="Q1" s="118">
         <v>45530</v>
       </c>
-      <c r="R1" s="115"/>
-      <c r="S1" s="115"/>
-      <c r="T1" s="115"/>
-      <c r="U1" s="115"/>
-      <c r="V1" s="115"/>
-      <c r="W1" s="115"/>
-      <c r="X1" s="115"/>
-      <c r="Y1" s="115"/>
-      <c r="Z1" s="115"/>
+      <c r="R1" s="117"/>
+      <c r="S1" s="117"/>
+      <c r="T1" s="117"/>
+      <c r="U1" s="117"/>
+      <c r="V1" s="117"/>
+      <c r="W1" s="117"/>
+      <c r="X1" s="117"/>
+      <c r="Y1" s="117"/>
+      <c r="Z1" s="117"/>
     </row>
     <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B2" s="93" t="s">
@@ -1846,28 +1846,28 @@
       <c r="D2" s="22"/>
       <c r="E2" s="23"/>
       <c r="F2" s="22"/>
-      <c r="I2" s="117" t="s">
+      <c r="I2" s="119" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="118"/>
-      <c r="K2" s="118"/>
-      <c r="L2" s="118"/>
-      <c r="M2" s="118"/>
-      <c r="N2" s="118"/>
-      <c r="O2" s="118"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="120"/>
+      <c r="L2" s="120"/>
+      <c r="M2" s="120"/>
+      <c r="N2" s="120"/>
+      <c r="O2" s="120"/>
       <c r="P2" s="24"/>
-      <c r="Q2" s="114">
+      <c r="Q2" s="116">
         <v>14</v>
       </c>
-      <c r="R2" s="115"/>
-      <c r="S2" s="115"/>
-      <c r="T2" s="115"/>
-      <c r="U2" s="115"/>
-      <c r="V2" s="115"/>
-      <c r="W2" s="115"/>
-      <c r="X2" s="115"/>
-      <c r="Y2" s="115"/>
-      <c r="Z2" s="115"/>
+      <c r="R2" s="117"/>
+      <c r="S2" s="117"/>
+      <c r="T2" s="117"/>
+      <c r="U2" s="117"/>
+      <c r="V2" s="117"/>
+      <c r="W2" s="117"/>
+      <c r="X2" s="117"/>
+      <c r="Y2" s="117"/>
+      <c r="Z2" s="117"/>
     </row>
     <row r="3" spans="1:64" s="25" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13"/>
@@ -1885,102 +1885,102 @@
       </c>
       <c r="C4" s="35"/>
       <c r="E4" s="28"/>
-      <c r="I4" s="111">
+      <c r="I4" s="123">
         <f>I5</f>
         <v>45621</v>
       </c>
-      <c r="J4" s="109"/>
-      <c r="K4" s="109"/>
-      <c r="L4" s="109"/>
-      <c r="M4" s="109"/>
-      <c r="N4" s="109"/>
-      <c r="O4" s="109"/>
-      <c r="P4" s="109">
+      <c r="J4" s="121"/>
+      <c r="K4" s="121"/>
+      <c r="L4" s="121"/>
+      <c r="M4" s="121"/>
+      <c r="N4" s="121"/>
+      <c r="O4" s="121"/>
+      <c r="P4" s="121">
         <f>P5</f>
         <v>45628</v>
       </c>
-      <c r="Q4" s="109"/>
-      <c r="R4" s="109"/>
-      <c r="S4" s="109"/>
-      <c r="T4" s="109"/>
-      <c r="U4" s="109"/>
-      <c r="V4" s="109"/>
-      <c r="W4" s="109">
+      <c r="Q4" s="121"/>
+      <c r="R4" s="121"/>
+      <c r="S4" s="121"/>
+      <c r="T4" s="121"/>
+      <c r="U4" s="121"/>
+      <c r="V4" s="121"/>
+      <c r="W4" s="121">
         <f>W5</f>
         <v>45635</v>
       </c>
-      <c r="X4" s="109"/>
-      <c r="Y4" s="109"/>
-      <c r="Z4" s="109"/>
-      <c r="AA4" s="109"/>
-      <c r="AB4" s="109"/>
-      <c r="AC4" s="109"/>
-      <c r="AD4" s="109">
+      <c r="X4" s="121"/>
+      <c r="Y4" s="121"/>
+      <c r="Z4" s="121"/>
+      <c r="AA4" s="121"/>
+      <c r="AB4" s="121"/>
+      <c r="AC4" s="121"/>
+      <c r="AD4" s="121">
         <f>AD5</f>
         <v>45642</v>
       </c>
-      <c r="AE4" s="109"/>
-      <c r="AF4" s="109"/>
-      <c r="AG4" s="109"/>
-      <c r="AH4" s="109"/>
-      <c r="AI4" s="109"/>
-      <c r="AJ4" s="109"/>
-      <c r="AK4" s="109">
+      <c r="AE4" s="121"/>
+      <c r="AF4" s="121"/>
+      <c r="AG4" s="121"/>
+      <c r="AH4" s="121"/>
+      <c r="AI4" s="121"/>
+      <c r="AJ4" s="121"/>
+      <c r="AK4" s="121">
         <f>AK5</f>
         <v>45649</v>
       </c>
-      <c r="AL4" s="109"/>
-      <c r="AM4" s="109"/>
-      <c r="AN4" s="109"/>
-      <c r="AO4" s="109"/>
-      <c r="AP4" s="109"/>
-      <c r="AQ4" s="109"/>
-      <c r="AR4" s="109">
+      <c r="AL4" s="121"/>
+      <c r="AM4" s="121"/>
+      <c r="AN4" s="121"/>
+      <c r="AO4" s="121"/>
+      <c r="AP4" s="121"/>
+      <c r="AQ4" s="121"/>
+      <c r="AR4" s="121">
         <f>AR5</f>
         <v>45656</v>
       </c>
-      <c r="AS4" s="109"/>
-      <c r="AT4" s="109"/>
-      <c r="AU4" s="109"/>
-      <c r="AV4" s="109"/>
-      <c r="AW4" s="109"/>
-      <c r="AX4" s="109"/>
-      <c r="AY4" s="109">
+      <c r="AS4" s="121"/>
+      <c r="AT4" s="121"/>
+      <c r="AU4" s="121"/>
+      <c r="AV4" s="121"/>
+      <c r="AW4" s="121"/>
+      <c r="AX4" s="121"/>
+      <c r="AY4" s="121">
         <f>AY5</f>
         <v>45663</v>
       </c>
-      <c r="AZ4" s="109"/>
-      <c r="BA4" s="109"/>
-      <c r="BB4" s="109"/>
-      <c r="BC4" s="109"/>
-      <c r="BD4" s="109"/>
-      <c r="BE4" s="109"/>
-      <c r="BF4" s="109">
+      <c r="AZ4" s="121"/>
+      <c r="BA4" s="121"/>
+      <c r="BB4" s="121"/>
+      <c r="BC4" s="121"/>
+      <c r="BD4" s="121"/>
+      <c r="BE4" s="121"/>
+      <c r="BF4" s="121">
         <f>BF5</f>
         <v>45670</v>
       </c>
-      <c r="BG4" s="109"/>
-      <c r="BH4" s="109"/>
-      <c r="BI4" s="109"/>
-      <c r="BJ4" s="109"/>
-      <c r="BK4" s="109"/>
-      <c r="BL4" s="110"/>
+      <c r="BG4" s="121"/>
+      <c r="BH4" s="121"/>
+      <c r="BI4" s="121"/>
+      <c r="BJ4" s="121"/>
+      <c r="BK4" s="121"/>
+      <c r="BL4" s="122"/>
     </row>
     <row r="5" spans="1:64" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="119"/>
-      <c r="B5" s="120" t="s">
+      <c r="A5" s="109"/>
+      <c r="B5" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="122" t="s">
+      <c r="C5" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="112" t="s">
+      <c r="D5" s="114" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="112" t="s">
+      <c r="E5" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="112" t="s">
+      <c r="F5" s="114" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="29">
@@ -2209,12 +2209,12 @@
       </c>
     </row>
     <row r="6" spans="1:64" s="25" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="119"/>
-      <c r="B6" s="121"/>
-      <c r="C6" s="123"/>
-      <c r="D6" s="113"/>
-      <c r="E6" s="113"/>
-      <c r="F6" s="113"/>
+      <c r="A6" s="109"/>
+      <c r="B6" s="111"/>
+      <c r="C6" s="113"/>
+      <c r="D6" s="115"/>
+      <c r="E6" s="115"/>
+      <c r="F6" s="115"/>
       <c r="I6" s="32" t="str">
         <f t="shared" ref="I6:AN6" si="3">LEFT(TEXT(I5,"ddd"),1)</f>
         <v>M</v>
@@ -5187,7 +5187,7 @@
         <v>28</v>
       </c>
       <c r="D44" s="81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E44" s="82">
         <v>45639</v>
@@ -5410,16 +5410,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="Q1:Z1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="I2:O2"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
@@ -5428,6 +5418,16 @@
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="Q1:Z1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D46">
     <cfRule type="dataBar" priority="23">
@@ -5656,23 +5656,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5988,29 +5977,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6037,9 +6026,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>